<commit_message>
modificartion langue content matrix
</commit_message>
<xml_diff>
--- a/Document/ContentMatrix_v1.3.xlsx
+++ b/Document/ContentMatrix_v1.3.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1322931\Documents\projet\Document\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1257837\Desktop\servider\Document\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -206,9 +206,6 @@
     <t>acceuil.menu.deconecter</t>
   </si>
   <si>
-    <t>[mes messages]</t>
-  </si>
-  <si>
     <t>2. Inscription</t>
   </si>
   <si>
@@ -242,9 +239,6 @@
     <t>inscription.textBox.rePassword</t>
   </si>
   <si>
-    <t>[Re-enter Password]</t>
-  </si>
-  <si>
     <t>inscription.textBox.prenom</t>
   </si>
   <si>
@@ -260,18 +254,12 @@
     <t>[Last Name]</t>
   </si>
   <si>
-    <t>[Nom de famille]</t>
-  </si>
-  <si>
     <t>inscription.textbox.address</t>
   </si>
   <si>
     <t>[Address]</t>
   </si>
   <si>
-    <t>[Adress]</t>
-  </si>
-  <si>
     <t>[Contry]</t>
   </si>
   <si>
@@ -296,12 +284,6 @@
     <t>[Ville]</t>
   </si>
   <si>
-    <t>[Zip code]</t>
-  </si>
-  <si>
-    <t>[Code postal]</t>
-  </si>
-  <si>
     <t>inscription.textBox.Codepostal</t>
   </si>
   <si>
@@ -314,9 +296,6 @@
     <t>[Business account]</t>
   </si>
   <si>
-    <t>[Profil d'affaire]</t>
-  </si>
-  <si>
     <t>[Service provider]</t>
   </si>
   <si>
@@ -416,12 +395,6 @@
     <t>profil.btn.cmt_client</t>
   </si>
   <si>
-    <t>[Commentaires sur les services]</t>
-  </si>
-  <si>
-    <t>[Comments on services]</t>
-  </si>
-  <si>
     <t>profil.btn.contacter</t>
   </si>
   <si>
@@ -452,9 +425,6 @@
     <t>header.menu.parametre</t>
   </si>
   <si>
-    <t>[Page d'accueil]</t>
-  </si>
-  <si>
     <t>[Profil]</t>
   </si>
   <si>
@@ -506,9 +476,6 @@
     <t>7.R_Password</t>
   </si>
   <si>
-    <t>[Récupération de mot de passe]</t>
-  </si>
-  <si>
     <t>[Veuillez entrer le courriel utilisé pour votre inscription]</t>
   </si>
   <si>
@@ -716,9 +683,6 @@
     <t>[Déconnexion]</t>
   </si>
   <si>
-    <t>[Retaper le mot passe]</t>
-  </si>
-  <si>
     <t>[État/Province]</t>
   </si>
   <si>
@@ -728,12 +692,6 @@
     <t>[Mot de passe oublié?]</t>
   </si>
   <si>
-    <t>[Comments on customer]</t>
-  </si>
-  <si>
-    <t>[Commentaires sur le client]</t>
-  </si>
-  <si>
     <t>[Home]</t>
   </si>
   <si>
@@ -779,9 +737,6 @@
     <t>Informe l'utilisateur qu'il doit choisir son nouveau mot de passe</t>
   </si>
   <si>
-    <t>[Please type your new password]</t>
-  </si>
-  <si>
     <t>[Veuillez entrer votre nouveau mot de passe]</t>
   </si>
   <si>
@@ -797,18 +752,9 @@
     <t>Demande à l'utilisateur de réentrer son nouveau mot de passe</t>
   </si>
   <si>
-    <t>[New Password]</t>
-  </si>
-  <si>
     <t>[Nouveau mot de passe]</t>
   </si>
   <si>
-    <t>[Confirmez le mot de passe]</t>
-  </si>
-  <si>
-    <t>[Confirm password]</t>
-  </si>
-  <si>
     <t>Reinit_Password.btn.confirmer</t>
   </si>
   <si>
@@ -819,6 +765,60 @@
   </si>
   <si>
     <t>[Réinitialiser]</t>
+  </si>
+  <si>
+    <t>[Accueil]</t>
+  </si>
+  <si>
+    <t>Confirmer le mot passe]</t>
+  </si>
+  <si>
+    <t>[Confirm Password]</t>
+  </si>
+  <si>
+    <t>[Nom]</t>
+  </si>
+  <si>
+    <t>[Adresse]</t>
+  </si>
+  <si>
+    <t>[Postal/ZIP code]</t>
+  </si>
+  <si>
+    <t>[Code postal/ZIP]</t>
+  </si>
+  <si>
+    <t>[Profil d'affaires]</t>
+  </si>
+  <si>
+    <t>[S'inscrire]</t>
+  </si>
+  <si>
+    <t>[Services comments]</t>
+  </si>
+  <si>
+    <t>[Customer comments]</t>
+  </si>
+  <si>
+    <t>[Commentaires en tant que client]</t>
+  </si>
+  <si>
+    <t>[Commentaire sur les services]</t>
+  </si>
+  <si>
+    <t>[Please type in your new password]</t>
+  </si>
+  <si>
+    <t>[Confirmez le nouveau mot de passe]</t>
+  </si>
+  <si>
+    <t>[Confirm new password]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>[Récupération du mot de passe]</t>
   </si>
 </sst>
 </file>
@@ -828,11 +828,18 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yyyy;@"/>
   </numFmts>
-  <fonts count="30" x14ac:knownFonts="1">
+  <fonts count="31" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1287,43 +1294,43 @@
   </borders>
   <cellStyleXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="115">
+  <cellXfs count="117">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1353,25 +1360,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1380,13 +1387,13 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1395,121 +1402,121 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="17" fillId="9" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="18" fillId="9" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="13" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="14" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="17" fillId="13" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="13" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="14" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="14" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="18" fillId="9" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="19" fillId="9" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="15" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="15" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="11" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="11" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1518,37 +1525,37 @@
     <xf numFmtId="0" fontId="0" fillId="15" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="15" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="14" fillId="15" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="11" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="11" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="15" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1560,73 +1567,73 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="14" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="13" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="14" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="18" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="15" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="15" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="19" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -1638,29 +1645,35 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" xfId="31"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="11" xfId="31" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="20" borderId="11" xfId="31" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="11" xfId="31" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" xfId="31" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="20" borderId="11" xfId="31" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="11" xfId="31" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" xfId="31" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="32">
     <cellStyle name="20 % - Accent1" xfId="31" builtinId="30"/>
@@ -2081,11 +2094,11 @@
   <sheetData>
     <row r="1" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="112" t="s">
+      <c r="B2" s="113" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="112"/>
-      <c r="D2" s="112"/>
+      <c r="C2" s="113"/>
+      <c r="D2" s="113"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B4" s="101" t="s">
@@ -2267,7 +2280,7 @@
         <v>7</v>
       </c>
       <c r="B2" s="38" t="s">
-        <v>236</v>
+        <v>222</v>
       </c>
       <c r="C2" s="39"/>
     </row>
@@ -2285,7 +2298,7 @@
         <v>35</v>
       </c>
       <c r="B4" s="38" t="s">
-        <v>237</v>
+        <v>223</v>
       </c>
       <c r="C4" s="39"/>
     </row>
@@ -2303,9 +2316,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R857"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="R51" sqref="R51"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K47" sqref="K47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2395,25 +2408,25 @@
       </c>
       <c r="D2" s="70"/>
       <c r="E2" s="85" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
       <c r="F2" s="32" t="s">
         <v>39</v>
       </c>
       <c r="G2" s="55" t="s">
-        <v>204</v>
+        <v>193</v>
       </c>
       <c r="H2" s="55" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I2" s="55" t="s">
         <v>43</v>
       </c>
-      <c r="J2" s="111" t="s">
-        <v>149</v>
-      </c>
-      <c r="K2" s="111" t="s">
-        <v>153</v>
+      <c r="J2" s="110" t="s">
+        <v>139</v>
+      </c>
+      <c r="K2" s="110" t="s">
+        <v>143</v>
       </c>
       <c r="L2" s="60"/>
       <c r="M2" s="60"/>
@@ -2423,7 +2436,7 @@
         <v>53</v>
       </c>
       <c r="Q2" s="80" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
       <c r="R2" s="70"/>
     </row>
@@ -2437,35 +2450,35 @@
       </c>
       <c r="D3" s="70"/>
       <c r="E3" s="85" t="s">
-        <v>171</v>
+        <v>160</v>
       </c>
       <c r="F3" s="32" t="s">
         <v>39</v>
       </c>
       <c r="G3" s="55" t="s">
-        <v>203</v>
+        <v>192</v>
       </c>
       <c r="H3" s="55" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I3" s="55" t="s">
         <v>43</v>
       </c>
-      <c r="J3" s="113" t="s">
-        <v>225</v>
-      </c>
-      <c r="K3" s="113" t="s">
-        <v>226</v>
+      <c r="J3" s="111" t="s">
+        <v>214</v>
+      </c>
+      <c r="K3" s="111" t="s">
+        <v>215</v>
       </c>
       <c r="L3" s="60"/>
       <c r="M3" s="60"/>
       <c r="N3" s="60"/>
       <c r="O3" s="60"/>
       <c r="P3" s="16" t="s">
-        <v>240</v>
+        <v>226</v>
       </c>
       <c r="Q3" s="80" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
       <c r="R3" s="70"/>
     </row>
@@ -2481,25 +2494,25 @@
         <v>57</v>
       </c>
       <c r="E4" s="27" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="F4" s="25" t="s">
         <v>39</v>
       </c>
       <c r="G4" s="27" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="H4" s="55" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I4" s="27" t="s">
         <v>44</v>
       </c>
       <c r="J4" s="40" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="K4" s="40" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="L4" s="28"/>
       <c r="M4" s="28"/>
@@ -2509,7 +2522,7 @@
         <v>53</v>
       </c>
       <c r="Q4" s="80" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
       <c r="R4" s="34"/>
     </row>
@@ -2531,19 +2544,19 @@
         <v>39</v>
       </c>
       <c r="G5" s="27" t="s">
-        <v>200</v>
+        <v>189</v>
       </c>
       <c r="H5" s="55" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I5" s="27" t="s">
         <v>44</v>
       </c>
       <c r="J5" s="40" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="K5" s="40" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="L5" s="28"/>
       <c r="M5" s="28"/>
@@ -2553,7 +2566,7 @@
         <v>53</v>
       </c>
       <c r="Q5" s="80" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
       <c r="R5" s="34"/>
     </row>
@@ -2575,19 +2588,19 @@
         <v>39</v>
       </c>
       <c r="G6" s="27" t="s">
-        <v>201</v>
+        <v>190</v>
       </c>
       <c r="H6" s="55" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I6" s="27" t="s">
         <v>44</v>
       </c>
       <c r="J6" s="40" t="s">
-        <v>227</v>
+        <v>216</v>
       </c>
       <c r="K6" s="40" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="L6" s="28"/>
       <c r="M6" s="28"/>
@@ -2597,7 +2610,7 @@
         <v>53</v>
       </c>
       <c r="Q6" s="80" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
       <c r="R6" s="34"/>
     </row>
@@ -2619,19 +2632,19 @@
         <v>39</v>
       </c>
       <c r="G7" s="27" t="s">
-        <v>202</v>
+        <v>191</v>
       </c>
       <c r="H7" s="55" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I7" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="J7" s="114" t="s">
-        <v>219</v>
-      </c>
-      <c r="K7" s="109" t="s">
-        <v>59</v>
+      <c r="J7" s="112" t="s">
+        <v>208</v>
+      </c>
+      <c r="K7" s="114" t="s">
+        <v>133</v>
       </c>
       <c r="L7" s="28"/>
       <c r="M7" s="28"/>
@@ -2641,7 +2654,7 @@
         <v>53</v>
       </c>
       <c r="Q7" s="80" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
       <c r="R7" s="34"/>
     </row>
@@ -2663,19 +2676,19 @@
         <v>39</v>
       </c>
       <c r="G8" s="27" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="H8" s="55" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I8" s="27" t="s">
         <v>44</v>
       </c>
       <c r="J8" s="40" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
       <c r="K8" s="40" t="s">
-        <v>228</v>
+        <v>217</v>
       </c>
       <c r="L8" s="28"/>
       <c r="M8" s="28"/>
@@ -2685,39 +2698,39 @@
         <v>53</v>
       </c>
       <c r="Q8" s="80" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
       <c r="R8" s="34"/>
     </row>
     <row r="9" spans="1:18" s="18" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="36"/>
       <c r="B9" s="27" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C9" s="43">
         <v>2</v>
       </c>
       <c r="D9" s="33"/>
       <c r="E9" s="35" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F9" s="32" t="s">
         <v>39</v>
       </c>
       <c r="G9" s="27" t="s">
-        <v>198</v>
+        <v>187</v>
       </c>
       <c r="H9" s="55" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I9" s="27" t="s">
         <v>43</v>
       </c>
       <c r="J9" s="40" t="s">
+        <v>63</v>
+      </c>
+      <c r="K9" s="40" t="s">
         <v>64</v>
-      </c>
-      <c r="K9" s="40" t="s">
-        <v>65</v>
       </c>
       <c r="L9" s="28"/>
       <c r="M9" s="28"/>
@@ -2727,39 +2740,39 @@
         <v>53</v>
       </c>
       <c r="Q9" s="80" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
       <c r="R9" s="34"/>
     </row>
     <row r="10" spans="1:18" s="18" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="36"/>
       <c r="B10" s="27" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C10" s="43">
         <v>2</v>
       </c>
       <c r="D10" s="34"/>
       <c r="E10" s="27" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F10" s="32" t="s">
         <v>39</v>
       </c>
       <c r="G10" s="27" t="s">
-        <v>172</v>
+        <v>161</v>
       </c>
       <c r="H10" s="55" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I10" s="27" t="s">
         <v>43</v>
       </c>
       <c r="J10" s="40" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K10" s="40" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="L10" s="28"/>
       <c r="M10" s="28"/>
@@ -2769,39 +2782,39 @@
         <v>53</v>
       </c>
       <c r="Q10" s="80" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
       <c r="R10" s="34"/>
     </row>
     <row r="11" spans="1:18" s="18" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="36"/>
       <c r="B11" s="27" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C11" s="43">
         <v>2</v>
       </c>
       <c r="D11" s="34"/>
       <c r="E11" s="27" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F11" s="32" t="s">
         <v>39</v>
       </c>
       <c r="G11" s="27" t="s">
-        <v>176</v>
+        <v>165</v>
       </c>
       <c r="H11" s="55" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I11" s="27" t="s">
         <v>43</v>
       </c>
       <c r="J11" s="40" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="K11" s="40" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
       <c r="L11" s="28"/>
       <c r="M11" s="28"/>
@@ -2811,39 +2824,39 @@
         <v>53</v>
       </c>
       <c r="Q11" s="80" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
       <c r="R11" s="34"/>
     </row>
     <row r="12" spans="1:18" s="18" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="36"/>
       <c r="B12" s="27" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C12" s="43">
         <v>2</v>
       </c>
       <c r="D12" s="34"/>
       <c r="E12" s="30" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F12" s="32" t="s">
         <v>39</v>
       </c>
       <c r="G12" s="27" t="s">
-        <v>177</v>
+        <v>166</v>
       </c>
       <c r="H12" s="55" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I12" s="27" t="s">
         <v>43</v>
       </c>
       <c r="J12" s="40" t="s">
-        <v>71</v>
+        <v>248</v>
       </c>
       <c r="K12" s="40" t="s">
-        <v>229</v>
+        <v>247</v>
       </c>
       <c r="L12" s="28"/>
       <c r="M12" s="28"/>
@@ -2853,39 +2866,39 @@
         <v>53</v>
       </c>
       <c r="Q12" s="80" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
       <c r="R12" s="34"/>
     </row>
-    <row r="13" spans="1:18" s="18" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" s="18" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="36"/>
       <c r="B13" s="27" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C13" s="43">
         <v>2</v>
       </c>
       <c r="D13" s="34"/>
       <c r="E13" s="39" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F13" s="32" t="s">
         <v>39</v>
       </c>
       <c r="G13" s="27" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
       <c r="H13" s="55" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I13" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="J13" s="109" t="s">
-        <v>74</v>
+      <c r="J13" s="116" t="s">
+        <v>72</v>
       </c>
       <c r="K13" s="108" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="L13" s="28"/>
       <c r="M13" s="28"/>
@@ -2895,39 +2908,39 @@
         <v>53</v>
       </c>
       <c r="Q13" s="80" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
       <c r="R13" s="34"/>
     </row>
     <row r="14" spans="1:18" s="18" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="36"/>
       <c r="B14" s="27" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C14" s="43">
         <v>2</v>
       </c>
       <c r="D14" s="34"/>
       <c r="E14" s="34" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F14" s="32" t="s">
         <v>39</v>
       </c>
       <c r="G14" s="27" t="s">
-        <v>174</v>
+        <v>163</v>
       </c>
       <c r="H14" s="55" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I14" s="27" t="s">
         <v>43</v>
       </c>
       <c r="J14" s="40" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="K14" s="40" t="s">
-        <v>77</v>
+        <v>249</v>
       </c>
       <c r="L14" s="28"/>
       <c r="M14" s="28"/>
@@ -2937,39 +2950,39 @@
         <v>53</v>
       </c>
       <c r="Q14" s="80" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
       <c r="R14" s="34"/>
     </row>
     <row r="15" spans="1:18" s="18" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="36"/>
       <c r="B15" s="27" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C15" s="43">
         <v>2</v>
       </c>
       <c r="D15" s="34"/>
       <c r="E15" s="30" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="F15" s="32" t="s">
         <v>39</v>
       </c>
       <c r="G15" s="27" t="s">
-        <v>175</v>
+        <v>164</v>
       </c>
       <c r="H15" s="55" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I15" s="27" t="s">
         <v>43</v>
       </c>
       <c r="J15" s="40" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="K15" s="40" t="s">
-        <v>80</v>
+        <v>250</v>
       </c>
       <c r="L15" s="28"/>
       <c r="M15" s="28"/>
@@ -2979,39 +2992,39 @@
         <v>53</v>
       </c>
       <c r="Q15" s="80" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
       <c r="R15" s="34"/>
     </row>
     <row r="16" spans="1:18" s="18" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="36"/>
       <c r="B16" s="27" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C16" s="43">
         <v>2</v>
       </c>
       <c r="D16" s="34"/>
       <c r="E16" s="27" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="F16" s="32" t="s">
         <v>39</v>
       </c>
       <c r="G16" s="27" t="s">
-        <v>178</v>
+        <v>167</v>
       </c>
       <c r="H16" s="55" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I16" s="27" t="s">
         <v>43</v>
       </c>
       <c r="J16" s="40" t="s">
+        <v>77</v>
+      </c>
+      <c r="K16" s="40" t="s">
         <v>81</v>
-      </c>
-      <c r="K16" s="40" t="s">
-        <v>85</v>
       </c>
       <c r="L16" s="28"/>
       <c r="M16" s="28"/>
@@ -3021,39 +3034,39 @@
         <v>53</v>
       </c>
       <c r="Q16" s="80" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
       <c r="R16" s="34"/>
     </row>
     <row r="17" spans="1:18" s="18" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="36"/>
       <c r="B17" s="27" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C17" s="43">
         <v>2</v>
       </c>
       <c r="D17" s="34"/>
       <c r="E17" s="27" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="F17" s="32" t="s">
         <v>39</v>
       </c>
       <c r="G17" s="27" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
       <c r="H17" s="55" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I17" s="27" t="s">
         <v>43</v>
       </c>
       <c r="J17" s="40" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="K17" s="40" t="s">
-        <v>230</v>
+        <v>218</v>
       </c>
       <c r="L17" s="28"/>
       <c r="M17" s="28"/>
@@ -3063,39 +3076,39 @@
         <v>53</v>
       </c>
       <c r="Q17" s="80" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
       <c r="R17" s="34"/>
     </row>
     <row r="18" spans="1:18" s="18" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="36"/>
       <c r="B18" s="27" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C18" s="43">
         <v>2</v>
       </c>
       <c r="D18" s="34"/>
       <c r="E18" s="34" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="F18" s="32" t="s">
         <v>39</v>
       </c>
       <c r="G18" s="27" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
       <c r="H18" s="55" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I18" s="27" t="s">
         <v>43</v>
       </c>
       <c r="J18" s="40" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="K18" s="40" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="L18" s="28"/>
       <c r="M18" s="28"/>
@@ -3105,39 +3118,39 @@
         <v>53</v>
       </c>
       <c r="Q18" s="80" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
       <c r="R18" s="34"/>
     </row>
     <row r="19" spans="1:18" s="18" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="36"/>
       <c r="B19" s="27" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C19" s="43">
         <v>2</v>
       </c>
       <c r="D19" s="34"/>
       <c r="E19" s="34" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="F19" s="32" t="s">
         <v>39</v>
       </c>
       <c r="G19" s="27" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
       <c r="H19" s="55" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I19" s="27" t="s">
         <v>43</v>
       </c>
       <c r="J19" s="40" t="s">
-        <v>89</v>
+        <v>251</v>
       </c>
       <c r="K19" s="40" t="s">
-        <v>90</v>
+        <v>252</v>
       </c>
       <c r="L19" s="28"/>
       <c r="M19" s="28"/>
@@ -3147,39 +3160,39 @@
         <v>53</v>
       </c>
       <c r="Q19" s="80" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
       <c r="R19" s="34"/>
     </row>
     <row r="20" spans="1:18" s="18" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="36"/>
       <c r="B20" s="27" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C20" s="43">
         <v>2</v>
       </c>
       <c r="D20" s="31"/>
       <c r="E20" s="31" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="F20" s="32" t="s">
         <v>39</v>
       </c>
       <c r="G20" s="27" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="H20" s="55" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I20" s="27" t="s">
         <v>44</v>
       </c>
       <c r="J20" s="40" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="K20" s="40" t="s">
-        <v>154</v>
+        <v>144</v>
       </c>
       <c r="L20" s="28"/>
       <c r="M20" s="28"/>
@@ -3189,39 +3202,39 @@
         <v>53</v>
       </c>
       <c r="Q20" s="80" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
       <c r="R20" s="34"/>
     </row>
     <row r="21" spans="1:18" s="18" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="36"/>
       <c r="B21" s="27" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C21" s="43">
         <v>2</v>
       </c>
       <c r="D21" s="34"/>
       <c r="E21" s="30" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
       <c r="F21" s="32" t="s">
         <v>39</v>
       </c>
       <c r="G21" s="27" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
       <c r="H21" s="55" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I21" s="27" t="s">
         <v>44</v>
       </c>
       <c r="J21" s="40" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="K21" s="40" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="L21" s="28"/>
       <c r="M21" s="28"/>
@@ -3231,39 +3244,39 @@
         <v>53</v>
       </c>
       <c r="Q21" s="80" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
       <c r="R21" s="34"/>
     </row>
     <row r="22" spans="1:18" s="18" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="36"/>
       <c r="B22" s="27" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C22" s="43">
         <v>2</v>
       </c>
       <c r="D22" s="34"/>
       <c r="E22" s="39" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="F22" s="32" t="s">
         <v>39</v>
       </c>
       <c r="G22" s="27" t="s">
-        <v>205</v>
+        <v>194</v>
       </c>
       <c r="H22" s="55" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I22" s="27" t="s">
         <v>43</v>
       </c>
       <c r="J22" s="40" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="K22" s="40" t="s">
-        <v>95</v>
+        <v>253</v>
       </c>
       <c r="L22" s="28"/>
       <c r="M22" s="28"/>
@@ -3273,39 +3286,39 @@
         <v>53</v>
       </c>
       <c r="Q22" s="80" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
       <c r="R22" s="34"/>
     </row>
     <row r="23" spans="1:18" s="18" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="36"/>
       <c r="B23" s="27" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C23" s="43">
         <v>2</v>
       </c>
       <c r="D23" s="34"/>
       <c r="E23" s="27" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="F23" s="32" t="s">
         <v>39</v>
       </c>
       <c r="G23" s="27" t="s">
-        <v>206</v>
+        <v>195</v>
       </c>
       <c r="H23" s="55" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I23" s="27" t="s">
         <v>43</v>
       </c>
       <c r="J23" s="40" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="K23" s="40" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="L23" s="28"/>
       <c r="M23" s="28"/>
@@ -3315,39 +3328,39 @@
         <v>53</v>
       </c>
       <c r="Q23" s="80" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
       <c r="R23" s="34"/>
     </row>
     <row r="24" spans="1:18" s="18" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="36"/>
       <c r="B24" s="27" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C24" s="43">
         <v>2</v>
       </c>
       <c r="D24" s="34"/>
       <c r="E24" s="39" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="F24" s="32" t="s">
         <v>39</v>
       </c>
       <c r="G24" s="27" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
       <c r="H24" s="55" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I24" s="27" t="s">
         <v>44</v>
       </c>
       <c r="J24" s="40" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="K24" s="40" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="L24" s="28"/>
       <c r="M24" s="28"/>
@@ -3357,39 +3370,39 @@
         <v>53</v>
       </c>
       <c r="Q24" s="80" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
       <c r="R24" s="34"/>
     </row>
     <row r="25" spans="1:18" s="18" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="36"/>
       <c r="B25" s="27" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="C25" s="43">
         <v>3</v>
       </c>
       <c r="D25" s="34"/>
       <c r="E25" s="39" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="F25" s="32" t="s">
         <v>39</v>
       </c>
       <c r="G25" s="27" t="s">
-        <v>192</v>
+        <v>181</v>
       </c>
       <c r="H25" s="55" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I25" s="27" t="s">
         <v>43</v>
       </c>
       <c r="J25" s="40" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="K25" s="40" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
       <c r="L25" s="28"/>
       <c r="M25" s="28"/>
@@ -3399,30 +3412,30 @@
         <v>53</v>
       </c>
       <c r="Q25" s="80" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
       <c r="R25" s="34"/>
     </row>
     <row r="26" spans="1:18" s="18" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="36"/>
       <c r="B26" s="27" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="C26" s="43">
         <v>3</v>
       </c>
       <c r="D26" s="33"/>
       <c r="E26" s="35" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="F26" s="32" t="s">
         <v>39</v>
       </c>
       <c r="G26" s="27" t="s">
-        <v>191</v>
+        <v>180</v>
       </c>
       <c r="H26" s="55" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I26" s="27" t="s">
         <v>43</v>
@@ -3443,39 +3456,39 @@
         <v>53</v>
       </c>
       <c r="Q26" s="80" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
       <c r="R26" s="34"/>
     </row>
     <row r="27" spans="1:18" s="18" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="36"/>
       <c r="B27" s="27" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="C27" s="43">
         <v>3</v>
       </c>
       <c r="D27" s="34"/>
       <c r="E27" s="39" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="F27" s="32" t="s">
         <v>39</v>
       </c>
       <c r="G27" s="27" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
       <c r="H27" s="55" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I27" s="27" t="s">
         <v>43</v>
       </c>
       <c r="J27" s="40" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="K27" s="40" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="L27" s="28"/>
       <c r="M27" s="28"/>
@@ -3485,39 +3498,39 @@
         <v>53</v>
       </c>
       <c r="Q27" s="80" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
       <c r="R27" s="34"/>
     </row>
     <row r="28" spans="1:18" s="18" customFormat="1" ht="66.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="36"/>
       <c r="B28" s="27" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="C28" s="43">
         <v>3</v>
       </c>
       <c r="D28" s="34"/>
       <c r="E28" s="34" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="F28" s="32" t="s">
         <v>39</v>
       </c>
       <c r="G28" s="27" t="s">
-        <v>207</v>
+        <v>196</v>
       </c>
       <c r="H28" s="55" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I28" s="27" t="s">
         <v>43</v>
       </c>
       <c r="J28" s="40" t="s">
-        <v>231</v>
+        <v>219</v>
       </c>
       <c r="K28" s="40" t="s">
-        <v>232</v>
+        <v>220</v>
       </c>
       <c r="L28" s="28"/>
       <c r="M28" s="28"/>
@@ -3527,39 +3540,39 @@
         <v>53</v>
       </c>
       <c r="Q28" s="80" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
       <c r="R28" s="34"/>
     </row>
     <row r="29" spans="1:18" s="18" customFormat="1" ht="66.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="36"/>
       <c r="B29" s="27" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="C29" s="43">
         <v>3</v>
       </c>
       <c r="D29" s="34"/>
       <c r="E29" s="39" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="F29" s="32" t="s">
         <v>39</v>
       </c>
       <c r="G29" s="27" t="s">
-        <v>208</v>
+        <v>197</v>
       </c>
       <c r="H29" s="55" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I29" s="27" t="s">
         <v>43</v>
       </c>
       <c r="J29" s="40" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="K29" s="40" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="L29" s="28"/>
       <c r="M29" s="28"/>
@@ -3569,39 +3582,39 @@
         <v>53</v>
       </c>
       <c r="Q29" s="80" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
       <c r="R29" s="34"/>
     </row>
     <row r="30" spans="1:18" s="18" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="69"/>
       <c r="B30" s="27" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="C30" s="43">
         <v>3</v>
       </c>
       <c r="D30" s="70"/>
       <c r="E30" s="70" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="F30" s="32" t="s">
         <v>39</v>
       </c>
       <c r="G30" s="55" t="s">
-        <v>209</v>
+        <v>198</v>
       </c>
       <c r="H30" s="55" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I30" s="55" t="s">
         <v>43</v>
       </c>
       <c r="J30" s="40" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K30" s="40" t="s">
-        <v>65</v>
+        <v>254</v>
       </c>
       <c r="L30" s="60"/>
       <c r="M30" s="60"/>
@@ -3611,39 +3624,39 @@
         <v>53</v>
       </c>
       <c r="Q30" s="80" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
       <c r="R30" s="70"/>
     </row>
     <row r="31" spans="1:18" s="18" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="36"/>
       <c r="B31" s="27" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="C31" s="43">
         <v>3</v>
       </c>
       <c r="D31" s="34"/>
       <c r="E31" s="39" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="F31" s="32" t="s">
         <v>39</v>
       </c>
       <c r="G31" s="27" t="s">
-        <v>189</v>
+        <v>178</v>
       </c>
       <c r="H31" s="55" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I31" s="27" t="s">
         <v>43</v>
       </c>
       <c r="J31" s="40" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="K31" s="40" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="L31" s="28"/>
       <c r="M31" s="28"/>
@@ -3653,39 +3666,39 @@
         <v>53</v>
       </c>
       <c r="Q31" s="80" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
       <c r="R31" s="34"/>
     </row>
     <row r="32" spans="1:18" s="18" customFormat="1" ht="57" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="36"/>
       <c r="B32" s="27" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="C32" s="43">
         <v>4</v>
       </c>
       <c r="D32" s="34"/>
       <c r="E32" s="39" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="F32" s="37" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="G32" s="27" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
       <c r="H32" s="55" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I32" s="27" t="s">
         <v>43</v>
       </c>
       <c r="J32" s="40" t="s">
-        <v>220</v>
+        <v>209</v>
       </c>
       <c r="K32" s="40" t="s">
-        <v>221</v>
+        <v>210</v>
       </c>
       <c r="L32" s="28"/>
       <c r="M32" s="28"/>
@@ -3695,39 +3708,39 @@
         <v>53</v>
       </c>
       <c r="Q32" s="80" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
       <c r="R32" s="34"/>
     </row>
     <row r="33" spans="1:18" s="18" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A33" s="36"/>
       <c r="B33" s="27" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="C33" s="43">
         <v>4</v>
       </c>
       <c r="D33" s="34"/>
       <c r="E33" s="34" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="F33" s="37" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="G33" s="27" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="H33" s="55" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I33" s="27" t="s">
         <v>43</v>
       </c>
       <c r="J33" s="40" t="s">
-        <v>222</v>
+        <v>211</v>
       </c>
       <c r="K33" s="40" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="L33" s="28"/>
       <c r="M33" s="28"/>
@@ -3737,39 +3750,39 @@
         <v>53</v>
       </c>
       <c r="Q33" s="80" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
       <c r="R33" s="34"/>
     </row>
     <row r="34" spans="1:18" s="18" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="36"/>
       <c r="B34" s="27" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="C34" s="43">
         <v>5</v>
       </c>
       <c r="D34" s="34"/>
       <c r="E34" s="30" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="F34" s="37" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="G34" s="27" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="H34" s="55" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I34" s="27" t="s">
         <v>43</v>
       </c>
       <c r="J34" s="40" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="K34" s="40" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="L34" s="28"/>
       <c r="M34" s="28"/>
@@ -3779,39 +3792,39 @@
         <v>53</v>
       </c>
       <c r="Q34" s="80" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
       <c r="R34" s="34"/>
     </row>
     <row r="35" spans="1:18" s="18" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="36"/>
       <c r="B35" s="27" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="C35" s="43">
         <v>5</v>
       </c>
       <c r="D35" s="34"/>
       <c r="E35" s="34" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="F35" s="37" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="G35" s="27" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="H35" s="55" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I35" s="27" t="s">
         <v>43</v>
       </c>
       <c r="J35" s="40" t="s">
-        <v>130</v>
+        <v>255</v>
       </c>
       <c r="K35" s="40" t="s">
-        <v>129</v>
+        <v>258</v>
       </c>
       <c r="L35" s="28"/>
       <c r="M35" s="28"/>
@@ -3821,39 +3834,39 @@
         <v>53</v>
       </c>
       <c r="Q35" s="80" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
       <c r="R35" s="34"/>
     </row>
     <row r="36" spans="1:18" s="18" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="36"/>
       <c r="B36" s="27" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="C36" s="43">
         <v>5</v>
       </c>
       <c r="D36" s="34"/>
       <c r="E36" s="27" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="F36" s="37" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="G36" s="27" t="s">
-        <v>210</v>
+        <v>199</v>
       </c>
       <c r="H36" s="55" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I36" s="27" t="s">
         <v>43</v>
       </c>
       <c r="J36" s="40" t="s">
-        <v>233</v>
+        <v>256</v>
       </c>
       <c r="K36" s="40" t="s">
-        <v>234</v>
+        <v>257</v>
       </c>
       <c r="L36" s="28"/>
       <c r="M36" s="28"/>
@@ -3863,39 +3876,39 @@
         <v>53</v>
       </c>
       <c r="Q36" s="80" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
       <c r="R36" s="34"/>
     </row>
     <row r="37" spans="1:18" s="18" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A37" s="36"/>
       <c r="B37" s="27" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="C37" s="43">
         <v>5</v>
       </c>
       <c r="D37" s="34"/>
       <c r="E37" s="39" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="F37" s="37" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="G37" s="27" t="s">
-        <v>211</v>
+        <v>200</v>
       </c>
       <c r="H37" s="55" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I37" s="27" t="s">
         <v>43</v>
       </c>
       <c r="J37" s="40" t="s">
-        <v>222</v>
+        <v>211</v>
       </c>
       <c r="K37" s="40" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="L37" s="28"/>
       <c r="M37" s="28"/>
@@ -3905,38 +3918,38 @@
         <v>53</v>
       </c>
       <c r="Q37" s="80" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
       <c r="R37" s="34"/>
     </row>
     <row r="38" spans="1:18" s="18" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="B38" s="27" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="C38" s="43">
         <v>6</v>
       </c>
       <c r="D38" s="34"/>
       <c r="E38" s="39" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="F38" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="G38" s="109" t="s">
+        <v>201</v>
+      </c>
+      <c r="H38" s="55" t="s">
         <v>62</v>
       </c>
-      <c r="G38" s="110" t="s">
-        <v>212</v>
-      </c>
-      <c r="H38" s="55" t="s">
-        <v>63</v>
-      </c>
-      <c r="I38" s="110" t="s">
+      <c r="I38" s="109" t="s">
         <v>43</v>
       </c>
-      <c r="J38" s="113" t="s">
-        <v>235</v>
-      </c>
-      <c r="K38" s="111" t="s">
-        <v>141</v>
+      <c r="J38" s="111" t="s">
+        <v>221</v>
+      </c>
+      <c r="K38" s="115" t="s">
+        <v>246</v>
       </c>
       <c r="L38" s="28"/>
       <c r="M38" s="28"/>
@@ -3946,39 +3959,39 @@
         <v>53</v>
       </c>
       <c r="Q38" s="80" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
       <c r="R38" s="34"/>
     </row>
     <row r="39" spans="1:18" s="18" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="36"/>
       <c r="B39" s="27" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="C39" s="43">
         <v>6</v>
       </c>
       <c r="D39" s="34"/>
       <c r="E39" s="30" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="F39" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="G39" s="27" t="s">
+        <v>202</v>
+      </c>
+      <c r="H39" s="55" t="s">
         <v>62</v>
-      </c>
-      <c r="G39" s="27" t="s">
-        <v>213</v>
-      </c>
-      <c r="H39" s="55" t="s">
-        <v>63</v>
       </c>
       <c r="I39" s="27" t="s">
         <v>43</v>
       </c>
       <c r="J39" s="40" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="K39" s="40" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="L39" s="28"/>
       <c r="M39" s="28"/>
@@ -3988,39 +4001,39 @@
         <v>53</v>
       </c>
       <c r="Q39" s="80" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
       <c r="R39" s="34"/>
     </row>
     <row r="40" spans="1:18" s="18" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="36"/>
       <c r="B40" s="27" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="C40" s="43">
         <v>6</v>
       </c>
       <c r="D40" s="34"/>
       <c r="E40" s="34" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="F40" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="G40" s="27" t="s">
+        <v>203</v>
+      </c>
+      <c r="H40" s="55" t="s">
         <v>62</v>
-      </c>
-      <c r="G40" s="27" t="s">
-        <v>214</v>
-      </c>
-      <c r="H40" s="55" t="s">
-        <v>63</v>
       </c>
       <c r="I40" s="27" t="s">
         <v>43</v>
       </c>
       <c r="J40" s="40" t="s">
-        <v>219</v>
+        <v>208</v>
       </c>
       <c r="K40" s="40" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="L40" s="28"/>
       <c r="M40" s="28"/>
@@ -4030,39 +4043,39 @@
         <v>53</v>
       </c>
       <c r="Q40" s="80" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
       <c r="R40" s="34"/>
     </row>
     <row r="41" spans="1:18" s="81" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="36"/>
       <c r="B41" s="27" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="C41" s="43">
         <v>6</v>
       </c>
       <c r="D41" s="34"/>
       <c r="E41" s="34" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="F41" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="G41" s="27" t="s">
+        <v>204</v>
+      </c>
+      <c r="H41" s="55" t="s">
         <v>62</v>
-      </c>
-      <c r="G41" s="27" t="s">
-        <v>215</v>
-      </c>
-      <c r="H41" s="55" t="s">
-        <v>63</v>
       </c>
       <c r="I41" s="27" t="s">
         <v>43</v>
       </c>
       <c r="J41" s="40" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
       <c r="K41" s="40" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="L41" s="28"/>
       <c r="M41" s="28"/>
@@ -4072,39 +4085,39 @@
         <v>53</v>
       </c>
       <c r="Q41" s="80" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
       <c r="R41" s="34"/>
     </row>
     <row r="42" spans="1:18" s="81" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A42" s="36"/>
       <c r="B42" s="27" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="C42" s="43">
         <v>6</v>
       </c>
       <c r="D42" s="34"/>
       <c r="E42" s="34" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="F42" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="G42" s="27" t="s">
+        <v>205</v>
+      </c>
+      <c r="H42" s="55" t="s">
         <v>62</v>
-      </c>
-      <c r="G42" s="27" t="s">
-        <v>216</v>
-      </c>
-      <c r="H42" s="55" t="s">
-        <v>63</v>
       </c>
       <c r="I42" s="27" t="s">
         <v>43</v>
       </c>
       <c r="J42" s="40" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
       <c r="K42" s="40" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="L42" s="28"/>
       <c r="M42" s="28"/>
@@ -4114,39 +4127,39 @@
         <v>53</v>
       </c>
       <c r="Q42" s="80" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
       <c r="R42" s="34"/>
     </row>
     <row r="43" spans="1:18" s="81" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="69"/>
       <c r="B43" s="55" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="C43" s="71">
         <v>6</v>
       </c>
       <c r="D43" s="70"/>
       <c r="E43" s="70" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="F43" s="32" t="s">
+        <v>61</v>
+      </c>
+      <c r="G43" s="27" t="s">
+        <v>175</v>
+      </c>
+      <c r="H43" s="55" t="s">
         <v>62</v>
-      </c>
-      <c r="G43" s="27" t="s">
-        <v>186</v>
-      </c>
-      <c r="H43" s="55" t="s">
-        <v>63</v>
       </c>
       <c r="I43" s="55" t="s">
         <v>43</v>
       </c>
       <c r="J43" s="40" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="K43" s="40" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="L43" s="60"/>
       <c r="M43" s="60"/>
@@ -4156,39 +4169,39 @@
         <v>53</v>
       </c>
       <c r="Q43" s="80" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
       <c r="R43" s="70"/>
     </row>
     <row r="44" spans="1:18" s="81" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="36"/>
       <c r="B44" s="27" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="C44" s="43">
         <v>6</v>
       </c>
       <c r="D44" s="34"/>
       <c r="E44" s="30" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
       <c r="F44" s="37" t="s">
         <v>39</v>
       </c>
       <c r="G44" s="27" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="H44" s="55" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I44" s="27" t="s">
         <v>43</v>
       </c>
       <c r="J44" s="40" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
       <c r="K44" s="40" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="L44" s="28"/>
       <c r="M44" s="28"/>
@@ -4198,27 +4211,27 @@
         <v>53</v>
       </c>
       <c r="Q44" s="80" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
       <c r="R44" s="34"/>
     </row>
     <row r="45" spans="1:18" s="81" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A45" s="36"/>
       <c r="B45" s="27" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="C45" s="43">
         <v>6</v>
       </c>
       <c r="D45" s="34"/>
       <c r="E45" s="30" t="s">
-        <v>238</v>
+        <v>224</v>
       </c>
       <c r="F45" s="37" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G45" s="27" t="s">
-        <v>239</v>
+        <v>225</v>
       </c>
       <c r="H45" s="55" t="s">
         <v>40</v>
@@ -4233,42 +4246,42 @@
       <c r="N45" s="28"/>
       <c r="O45" s="28"/>
       <c r="P45" s="25" t="s">
-        <v>240</v>
+        <v>226</v>
       </c>
       <c r="Q45" s="80" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
       <c r="R45" s="34"/>
     </row>
     <row r="46" spans="1:18" s="21" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A46" s="36"/>
       <c r="B46" s="27" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="C46" s="43">
         <v>7</v>
       </c>
       <c r="D46" s="34"/>
       <c r="E46" s="34" t="s">
-        <v>243</v>
+        <v>229</v>
       </c>
       <c r="F46" s="37" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="G46" s="27" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
       <c r="H46" s="55" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I46" s="27" t="s">
         <v>43</v>
       </c>
       <c r="J46" s="40" t="s">
-        <v>246</v>
+        <v>232</v>
       </c>
       <c r="K46" s="40" t="s">
-        <v>159</v>
+        <v>263</v>
       </c>
       <c r="L46" s="28"/>
       <c r="M46" s="28"/>
@@ -4278,39 +4291,39 @@
         <v>53</v>
       </c>
       <c r="Q46" s="80" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
       <c r="R46" s="34"/>
     </row>
     <row r="47" spans="1:18" s="18" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A47" s="36"/>
       <c r="B47" s="27" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="C47" s="43">
         <v>7</v>
       </c>
       <c r="D47" s="34"/>
       <c r="E47" s="30" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="F47" s="37" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="G47" s="27" t="s">
-        <v>218</v>
+        <v>207</v>
       </c>
       <c r="H47" s="55" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I47" s="27" t="s">
         <v>43</v>
       </c>
       <c r="J47" s="40" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
       <c r="K47" s="40" t="s">
-        <v>160</v>
+        <v>149</v>
       </c>
       <c r="L47" s="28"/>
       <c r="M47" s="28"/>
@@ -4320,39 +4333,39 @@
         <v>53</v>
       </c>
       <c r="Q47" s="80" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
       <c r="R47" s="34"/>
     </row>
     <row r="48" spans="1:18" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A48" s="36"/>
       <c r="B48" s="27" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="C48" s="43">
         <v>7</v>
       </c>
       <c r="D48" s="34"/>
       <c r="E48" s="34" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="F48" s="37" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="G48" s="27" t="s">
-        <v>192</v>
+        <v>181</v>
       </c>
       <c r="H48" s="55" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I48" s="27" t="s">
         <v>43</v>
       </c>
       <c r="J48" s="40" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="K48" s="40" t="s">
-        <v>162</v>
+        <v>151</v>
       </c>
       <c r="L48" s="28"/>
       <c r="M48" s="28"/>
@@ -4362,39 +4375,39 @@
         <v>53</v>
       </c>
       <c r="Q48" s="80" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
       <c r="R48" s="34"/>
     </row>
     <row r="49" spans="1:18" s="21" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A49" s="36"/>
       <c r="B49" s="27" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="C49" s="43">
         <v>7</v>
       </c>
       <c r="D49" s="34"/>
       <c r="E49" s="34" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
       <c r="F49" s="37" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="G49" s="27" t="s">
-        <v>217</v>
+        <v>206</v>
       </c>
       <c r="H49" s="55" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I49" s="27" t="s">
         <v>43</v>
       </c>
       <c r="J49" s="40" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="K49" s="40" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
       <c r="L49" s="28"/>
       <c r="M49" s="28"/>
@@ -4404,217 +4417,217 @@
         <v>53</v>
       </c>
       <c r="Q49" s="80" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
       <c r="R49" s="34"/>
     </row>
     <row r="50" spans="1:18" s="18" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="36"/>
       <c r="B50" s="27" t="s">
-        <v>241</v>
+        <v>227</v>
       </c>
       <c r="C50" s="43">
         <v>8</v>
       </c>
       <c r="D50" s="34"/>
       <c r="E50" s="27" t="s">
-        <v>242</v>
+        <v>228</v>
       </c>
       <c r="F50" s="37" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="G50" s="27" t="s">
-        <v>244</v>
+        <v>230</v>
       </c>
       <c r="H50" s="27" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I50" s="27" t="s">
         <v>43</v>
       </c>
       <c r="J50" s="40" t="s">
-        <v>247</v>
+        <v>233</v>
       </c>
       <c r="K50" s="40" t="s">
-        <v>245</v>
+        <v>231</v>
       </c>
       <c r="L50" s="28"/>
       <c r="M50" s="28"/>
       <c r="N50" s="28"/>
       <c r="O50" s="28"/>
       <c r="P50" s="25" t="s">
-        <v>240</v>
+        <v>226</v>
       </c>
       <c r="Q50" s="26" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
       <c r="R50" s="34"/>
     </row>
     <row r="51" spans="1:18" s="18" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="69"/>
       <c r="B51" s="55" t="s">
-        <v>241</v>
+        <v>227</v>
       </c>
       <c r="C51" s="71">
         <v>8</v>
       </c>
       <c r="D51" s="70"/>
       <c r="E51" s="55" t="s">
-        <v>248</v>
+        <v>234</v>
       </c>
       <c r="F51" s="32" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="G51" s="55" t="s">
-        <v>249</v>
+        <v>235</v>
       </c>
       <c r="H51" s="55" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I51" s="55" t="s">
         <v>43</v>
       </c>
       <c r="J51" s="40" t="s">
-        <v>250</v>
+        <v>259</v>
       </c>
       <c r="K51" s="40" t="s">
-        <v>251</v>
+        <v>236</v>
       </c>
       <c r="L51" s="60"/>
       <c r="M51" s="60"/>
       <c r="N51" s="60"/>
       <c r="O51" s="60"/>
       <c r="P51" s="16" t="s">
-        <v>240</v>
+        <v>226</v>
       </c>
       <c r="Q51" s="80" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
       <c r="R51" s="70"/>
     </row>
     <row r="52" spans="1:18" s="18" customFormat="1" ht="69" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="69"/>
       <c r="B52" s="55" t="s">
-        <v>241</v>
+        <v>227</v>
       </c>
       <c r="C52" s="71">
         <v>8</v>
       </c>
       <c r="D52" s="70"/>
       <c r="E52" s="55" t="s">
-        <v>252</v>
+        <v>237</v>
       </c>
       <c r="F52" s="32" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="G52" s="27" t="s">
-        <v>254</v>
+        <v>239</v>
       </c>
       <c r="H52" s="55" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I52" s="55" t="s">
         <v>43</v>
       </c>
       <c r="J52" s="93" t="s">
-        <v>256</v>
+        <v>262</v>
       </c>
       <c r="K52" s="93" t="s">
-        <v>257</v>
+        <v>241</v>
       </c>
       <c r="L52" s="95"/>
       <c r="M52" s="95"/>
       <c r="N52" s="95"/>
       <c r="O52" s="95"/>
       <c r="P52" s="96" t="s">
-        <v>240</v>
+        <v>226</v>
       </c>
       <c r="Q52" s="80" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
       <c r="R52" s="97"/>
     </row>
     <row r="53" spans="1:18" s="18" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="36"/>
       <c r="B53" s="27" t="s">
-        <v>241</v>
+        <v>227</v>
       </c>
       <c r="C53" s="43">
         <v>8</v>
       </c>
       <c r="D53" s="34"/>
       <c r="E53" s="55" t="s">
-        <v>253</v>
+        <v>238</v>
       </c>
       <c r="F53" s="32" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="G53" s="27" t="s">
-        <v>255</v>
+        <v>240</v>
       </c>
       <c r="H53" s="27" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I53" s="27" t="s">
         <v>43</v>
       </c>
       <c r="J53" s="40" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="K53" s="40" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="L53" s="28"/>
       <c r="M53" s="28"/>
       <c r="N53" s="28"/>
       <c r="O53" s="28"/>
       <c r="P53" s="25" t="s">
-        <v>240</v>
+        <v>226</v>
       </c>
       <c r="Q53" s="26" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
       <c r="R53" s="34"/>
     </row>
     <row r="54" spans="1:18" s="18" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="36"/>
       <c r="B54" s="27" t="s">
-        <v>241</v>
+        <v>227</v>
       </c>
       <c r="C54" s="43">
         <v>8</v>
       </c>
       <c r="D54" s="34"/>
       <c r="E54" s="39" t="s">
-        <v>260</v>
+        <v>242</v>
       </c>
       <c r="F54" s="37" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="G54" s="27" t="s">
-        <v>261</v>
+        <v>243</v>
       </c>
       <c r="H54" s="27" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I54" s="27" t="s">
         <v>43</v>
       </c>
       <c r="J54" s="40" t="s">
-        <v>262</v>
+        <v>244</v>
       </c>
       <c r="K54" s="40" t="s">
-        <v>263</v>
+        <v>245</v>
       </c>
       <c r="L54" s="28"/>
       <c r="M54" s="28"/>
       <c r="N54" s="28"/>
       <c r="O54" s="28"/>
       <c r="P54" s="25" t="s">
-        <v>240</v>
+        <v>226</v>
       </c>
       <c r="Q54" s="26" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
       <c r="R54" s="34"/>
     </row>
@@ -20631,18 +20644,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="B1" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
       <c r="B2" t="s">
-        <v>224</v>
+        <v>213</v>
       </c>
     </row>
   </sheetData>
@@ -20651,9 +20664,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -20706,24 +20722,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{30E84F96-43E5-4C3A-8E0E-76AD01F7D6A1}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{56277F14-5102-450B-9F74-CC1199F0A7EB}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -20744,9 +20751,15 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{56277F14-5102-450B-9F74-CC1199F0A7EB}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{30E84F96-43E5-4C3A-8E0E-76AD01F7D6A1}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
le magnifique conrtent matrix
</commit_message>
<xml_diff>
--- a/Document/ContentMatrix_v1.3.xlsx
+++ b/Document/ContentMatrix_v1.3.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1290" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="850" uniqueCount="357">
   <si>
     <t>VERSION</t>
   </si>
@@ -894,6 +894,210 @@
   </si>
   <si>
     <t>Message.lb.date</t>
+  </si>
+  <si>
+    <t>Parametre.lbl.parametre</t>
+  </si>
+  <si>
+    <t>[Parameter]</t>
+  </si>
+  <si>
+    <t>[Paramètre]</t>
+  </si>
+  <si>
+    <t>18-09-2015</t>
+  </si>
+  <si>
+    <t>11.Paramètre</t>
+  </si>
+  <si>
+    <t>Parametre.lbl.changermotpasse</t>
+  </si>
+  <si>
+    <t>le message changer le mot de passe</t>
+  </si>
+  <si>
+    <t>[Changer mot de passe]</t>
+  </si>
+  <si>
+    <t>[Change your password]</t>
+  </si>
+  <si>
+    <t>Parametre.hint.oldpassword</t>
+  </si>
+  <si>
+    <t>[Last password]</t>
+  </si>
+  <si>
+    <t>[Ancien mot de passe]</t>
+  </si>
+  <si>
+    <t>Parametre.hint.newpassword</t>
+  </si>
+  <si>
+    <t>invite a entrer  l'ancien mot de passe</t>
+  </si>
+  <si>
+    <t>invite a entrer le nouveau mot de passe</t>
+  </si>
+  <si>
+    <t>[New password]</t>
+  </si>
+  <si>
+    <t>Parametre.hint.confirmerpassword</t>
+  </si>
+  <si>
+    <t>invite a confirmer son password</t>
+  </si>
+  <si>
+    <t>[Confirm password]</t>
+  </si>
+  <si>
+    <t>[Confirmer mot de passe]</t>
+  </si>
+  <si>
+    <t>Parametre.btn.confirmerpassword</t>
+  </si>
+  <si>
+    <t>btn pout confirmer mot de passe</t>
+  </si>
+  <si>
+    <t>[apply]</t>
+  </si>
+  <si>
+    <t>[Comfirmer]</t>
+  </si>
+  <si>
+    <t>Parametre.lbl.changeAdress</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> lbl changer adresse</t>
+  </si>
+  <si>
+    <t>[change adress]</t>
+  </si>
+  <si>
+    <t>[Changer adresse]</t>
+  </si>
+  <si>
+    <t>Parametre.hint.address</t>
+  </si>
+  <si>
+    <t>invite a entrer son adresse</t>
+  </si>
+  <si>
+    <t>Parametre.hint.pay</t>
+  </si>
+  <si>
+    <t>[Pay]</t>
+  </si>
+  <si>
+    <t>invite a entrer</t>
+  </si>
+  <si>
+    <t>Parametre.lstbox.code postal</t>
+  </si>
+  <si>
+    <t>pour entrer son code postale</t>
+  </si>
+  <si>
+    <t>[Code Postal/ZIP code]</t>
+  </si>
+  <si>
+    <t>Parametre.hint.password</t>
+  </si>
+  <si>
+    <t>invite a entre sdo n mot de passe</t>
+  </si>
+  <si>
+    <t>[mot de passe]</t>
+  </si>
+  <si>
+    <t>Parametre.btn.comffirmerAdresse</t>
+  </si>
+  <si>
+    <t>boutton pour confirmer son addresse</t>
+  </si>
+  <si>
+    <t>Hguo Belhumeur</t>
+  </si>
+  <si>
+    <t>Parametre.changeradressecourielle</t>
+  </si>
+  <si>
+    <t>montre changer adresse courielle</t>
+  </si>
+  <si>
+    <t>ajout des content matrix de la page de parametre</t>
+  </si>
+  <si>
+    <t>[Change email]</t>
+  </si>
+  <si>
+    <t>[Changer adresse courrielle]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Parametre.hint email </t>
+  </si>
+  <si>
+    <t>[Aplly]</t>
+  </si>
+  <si>
+    <t>[Confirmer]</t>
+  </si>
+  <si>
+    <t>[Nouvelle adresse courrielle]</t>
+  </si>
+  <si>
+    <t>invite a entrer  new email</t>
+  </si>
+  <si>
+    <t>Parametre.btn comfirmeremail</t>
+  </si>
+  <si>
+    <t>bouton pon confirmer son nouveau mot de passe</t>
+  </si>
+  <si>
+    <t>[Notification]</t>
+  </si>
+  <si>
+    <t>Parametre.lbl.notification</t>
+  </si>
+  <si>
+    <t>Parametre.checkbox.notifemail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Notfication </t>
+  </si>
+  <si>
+    <t>Notfication par courielle</t>
+  </si>
+  <si>
+    <t>[Me notifier par courriel]</t>
+  </si>
+  <si>
+    <t>Parametre.checkbox.partexto</t>
+  </si>
+  <si>
+    <t>notifcation par textyo</t>
+  </si>
+  <si>
+    <t>[Send me notification via texto]</t>
+  </si>
+  <si>
+    <t>[Aend notification to me by email]</t>
+  </si>
+  <si>
+    <t>[Apply]</t>
+  </si>
+  <si>
+    <t>[New email]</t>
+  </si>
+  <si>
+    <t>[Postal code/ ZIP code]</t>
+  </si>
+  <si>
+    <t>[Me notifier par texto]</t>
   </si>
 </sst>
 </file>
@@ -2391,9 +2595,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R857"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A54" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q62" sqref="Q62"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K80" sqref="K80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5036,362 +5240,758 @@
     </row>
     <row r="63" spans="1:18" s="18" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="36"/>
-      <c r="B63" s="27"/>
-      <c r="C63" s="43"/>
+      <c r="B63" s="27" t="s">
+        <v>293</v>
+      </c>
+      <c r="C63" s="43">
+        <v>11</v>
+      </c>
       <c r="D63" s="34"/>
-      <c r="E63" s="30"/>
-      <c r="F63" s="37"/>
-      <c r="G63" s="27"/>
-      <c r="H63" s="27"/>
-      <c r="I63" s="27"/>
-      <c r="J63" s="40"/>
-      <c r="K63" s="40"/>
+      <c r="E63" s="30" t="s">
+        <v>289</v>
+      </c>
+      <c r="F63" s="37" t="s">
+        <v>111</v>
+      </c>
+      <c r="G63" s="27" t="s">
+        <v>283</v>
+      </c>
+      <c r="H63" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="I63" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="J63" s="40" t="s">
+        <v>290</v>
+      </c>
+      <c r="K63" s="40" t="s">
+        <v>291</v>
+      </c>
       <c r="L63" s="28"/>
       <c r="M63" s="28"/>
       <c r="N63" s="28"/>
       <c r="O63" s="28"/>
-      <c r="P63" s="25"/>
-      <c r="Q63" s="26"/>
+      <c r="P63" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q63" s="26" t="s">
+        <v>292</v>
+      </c>
       <c r="R63" s="34"/>
     </row>
     <row r="64" spans="1:18" s="18" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="36"/>
-      <c r="B64" s="27"/>
-      <c r="C64" s="43"/>
+      <c r="B64" s="27" t="s">
+        <v>293</v>
+      </c>
+      <c r="C64" s="43">
+        <v>11</v>
+      </c>
       <c r="D64" s="34"/>
-      <c r="E64" s="39"/>
-      <c r="F64" s="37"/>
-      <c r="G64" s="27"/>
-      <c r="H64" s="27"/>
-      <c r="I64" s="27"/>
-      <c r="J64" s="54"/>
-      <c r="K64" s="54"/>
+      <c r="E64" s="39" t="s">
+        <v>294</v>
+      </c>
+      <c r="F64" s="37" t="s">
+        <v>111</v>
+      </c>
+      <c r="G64" s="27" t="s">
+        <v>295</v>
+      </c>
+      <c r="H64" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="I64" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="J64" s="54" t="s">
+        <v>297</v>
+      </c>
+      <c r="K64" s="54" t="s">
+        <v>296</v>
+      </c>
       <c r="L64" s="28"/>
       <c r="M64" s="28"/>
       <c r="N64" s="28"/>
       <c r="O64" s="28"/>
-      <c r="P64" s="25"/>
-      <c r="Q64" s="26"/>
+      <c r="P64" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q64" s="26" t="s">
+        <v>292</v>
+      </c>
       <c r="R64" s="34"/>
     </row>
     <row r="65" spans="1:18" s="18" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="36"/>
-      <c r="B65" s="27"/>
-      <c r="C65" s="43"/>
+      <c r="B65" s="27" t="s">
+        <v>293</v>
+      </c>
+      <c r="C65" s="43">
+        <v>11</v>
+      </c>
       <c r="D65" s="34"/>
-      <c r="E65" s="39"/>
-      <c r="F65" s="37"/>
-      <c r="G65" s="27"/>
-      <c r="H65" s="27"/>
-      <c r="I65" s="27"/>
-      <c r="J65" s="54"/>
-      <c r="K65" s="54"/>
+      <c r="E65" s="39" t="s">
+        <v>298</v>
+      </c>
+      <c r="F65" s="37" t="s">
+        <v>111</v>
+      </c>
+      <c r="G65" s="27" t="s">
+        <v>302</v>
+      </c>
+      <c r="H65" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="I65" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="J65" s="54" t="s">
+        <v>299</v>
+      </c>
+      <c r="K65" s="54" t="s">
+        <v>300</v>
+      </c>
       <c r="L65" s="28"/>
       <c r="M65" s="28"/>
       <c r="N65" s="28"/>
       <c r="O65" s="28"/>
-      <c r="P65" s="25"/>
-      <c r="Q65" s="26"/>
+      <c r="P65" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q65" s="26" t="s">
+        <v>292</v>
+      </c>
       <c r="R65" s="34"/>
     </row>
     <row r="66" spans="1:18" s="18" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="36"/>
-      <c r="B66" s="27"/>
-      <c r="C66" s="43"/>
+      <c r="B66" s="27" t="s">
+        <v>293</v>
+      </c>
+      <c r="C66" s="43">
+        <v>11</v>
+      </c>
       <c r="D66" s="34"/>
-      <c r="E66" s="30"/>
-      <c r="F66" s="37"/>
-      <c r="G66" s="27"/>
-      <c r="H66" s="27"/>
-      <c r="I66" s="27"/>
-      <c r="J66" s="40"/>
-      <c r="K66" s="40"/>
+      <c r="E66" s="30" t="s">
+        <v>301</v>
+      </c>
+      <c r="F66" s="37" t="s">
+        <v>111</v>
+      </c>
+      <c r="G66" s="27" t="s">
+        <v>303</v>
+      </c>
+      <c r="H66" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="I66" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="J66" s="40" t="s">
+        <v>304</v>
+      </c>
+      <c r="K66" s="40" t="s">
+        <v>241</v>
+      </c>
       <c r="L66" s="28"/>
       <c r="M66" s="28"/>
       <c r="N66" s="28"/>
       <c r="O66" s="28"/>
-      <c r="P66" s="25"/>
-      <c r="Q66" s="26"/>
+      <c r="P66" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q66" s="26" t="s">
+        <v>292</v>
+      </c>
       <c r="R66" s="34"/>
     </row>
     <row r="67" spans="1:18" s="18" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="36"/>
-      <c r="B67" s="27"/>
-      <c r="C67" s="43"/>
+      <c r="B67" s="27" t="s">
+        <v>293</v>
+      </c>
+      <c r="C67" s="43">
+        <v>11</v>
+      </c>
       <c r="D67" s="34"/>
-      <c r="E67" s="39"/>
-      <c r="F67" s="37"/>
-      <c r="G67" s="27"/>
-      <c r="H67" s="27"/>
-      <c r="I67" s="27"/>
-      <c r="J67" s="40"/>
-      <c r="K67" s="40"/>
+      <c r="E67" s="39" t="s">
+        <v>305</v>
+      </c>
+      <c r="F67" s="37" t="s">
+        <v>111</v>
+      </c>
+      <c r="G67" s="27" t="s">
+        <v>306</v>
+      </c>
+      <c r="H67" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="I67" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="J67" s="40" t="s">
+        <v>307</v>
+      </c>
+      <c r="K67" s="40" t="s">
+        <v>308</v>
+      </c>
       <c r="L67" s="28"/>
       <c r="M67" s="28"/>
       <c r="N67" s="28"/>
       <c r="O67" s="28"/>
-      <c r="P67" s="25"/>
-      <c r="Q67" s="26"/>
+      <c r="P67" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q67" s="26" t="s">
+        <v>292</v>
+      </c>
       <c r="R67" s="34"/>
     </row>
     <row r="68" spans="1:18" s="18" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="36"/>
-      <c r="B68" s="27"/>
-      <c r="C68" s="43"/>
+      <c r="B68" s="27" t="s">
+        <v>293</v>
+      </c>
+      <c r="C68" s="43">
+        <v>11</v>
+      </c>
       <c r="D68" s="34"/>
-      <c r="E68" s="34"/>
-      <c r="F68" s="37"/>
-      <c r="G68" s="27"/>
-      <c r="H68" s="27"/>
-      <c r="I68" s="27"/>
-      <c r="J68" s="40"/>
-      <c r="K68" s="40"/>
+      <c r="E68" s="34" t="s">
+        <v>309</v>
+      </c>
+      <c r="F68" s="37" t="s">
+        <v>111</v>
+      </c>
+      <c r="G68" s="27" t="s">
+        <v>310</v>
+      </c>
+      <c r="H68" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="I68" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="J68" s="40" t="s">
+        <v>311</v>
+      </c>
+      <c r="K68" s="40" t="s">
+        <v>312</v>
+      </c>
       <c r="L68" s="28"/>
       <c r="M68" s="28"/>
       <c r="N68" s="28"/>
       <c r="O68" s="28"/>
-      <c r="P68" s="25"/>
-      <c r="Q68" s="26"/>
+      <c r="P68" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q68" s="26" t="s">
+        <v>292</v>
+      </c>
       <c r="R68" s="34"/>
     </row>
     <row r="69" spans="1:18" s="81" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="36"/>
-      <c r="B69" s="27"/>
-      <c r="C69" s="43"/>
+      <c r="B69" s="27" t="s">
+        <v>293</v>
+      </c>
+      <c r="C69" s="43">
+        <v>11</v>
+      </c>
       <c r="D69" s="34"/>
-      <c r="E69" s="34"/>
-      <c r="F69" s="37"/>
-      <c r="G69" s="27"/>
-      <c r="H69" s="27"/>
-      <c r="I69" s="27"/>
-      <c r="J69" s="40"/>
-      <c r="K69" s="40"/>
+      <c r="E69" s="34" t="s">
+        <v>313</v>
+      </c>
+      <c r="F69" s="37" t="s">
+        <v>111</v>
+      </c>
+      <c r="G69" s="27" t="s">
+        <v>314</v>
+      </c>
+      <c r="H69" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="I69" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="J69" s="40" t="s">
+        <v>315</v>
+      </c>
+      <c r="K69" s="40" t="s">
+        <v>316</v>
+      </c>
       <c r="L69" s="28"/>
       <c r="M69" s="28"/>
       <c r="N69" s="28"/>
       <c r="O69" s="28"/>
-      <c r="P69" s="25"/>
-      <c r="Q69" s="26"/>
+      <c r="P69" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q69" s="26" t="s">
+        <v>292</v>
+      </c>
       <c r="R69" s="34"/>
     </row>
     <row r="70" spans="1:18" s="81" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="36"/>
-      <c r="B70" s="27"/>
-      <c r="C70" s="43"/>
+      <c r="B70" s="27" t="s">
+        <v>293</v>
+      </c>
+      <c r="C70" s="43">
+        <v>11</v>
+      </c>
       <c r="D70" s="34"/>
-      <c r="E70" s="30"/>
-      <c r="F70" s="37"/>
-      <c r="G70" s="27"/>
-      <c r="H70" s="27"/>
-      <c r="I70" s="27"/>
-      <c r="J70" s="40"/>
-      <c r="K70" s="40"/>
+      <c r="E70" s="30" t="s">
+        <v>317</v>
+      </c>
+      <c r="F70" s="37" t="s">
+        <v>111</v>
+      </c>
+      <c r="G70" s="27" t="s">
+        <v>318</v>
+      </c>
+      <c r="H70" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="I70" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="J70" s="40" t="s">
+        <v>76</v>
+      </c>
+      <c r="K70" s="40" t="s">
+        <v>250</v>
+      </c>
       <c r="L70" s="28"/>
       <c r="M70" s="28"/>
       <c r="N70" s="28"/>
       <c r="O70" s="28"/>
-      <c r="P70" s="25"/>
-      <c r="Q70" s="26"/>
+      <c r="P70" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q70" s="26" t="s">
+        <v>292</v>
+      </c>
       <c r="R70" s="34"/>
     </row>
     <row r="71" spans="1:18" s="18" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="36"/>
-      <c r="B71" s="27"/>
-      <c r="C71" s="43"/>
+      <c r="B71" s="27" t="s">
+        <v>293</v>
+      </c>
+      <c r="C71" s="43">
+        <v>11</v>
+      </c>
       <c r="D71" s="27"/>
-      <c r="E71" s="34"/>
-      <c r="F71" s="37"/>
-      <c r="G71" s="27"/>
-      <c r="H71" s="27"/>
-      <c r="I71" s="27"/>
-      <c r="J71" s="40"/>
-      <c r="K71" s="40"/>
+      <c r="E71" s="34" t="s">
+        <v>319</v>
+      </c>
+      <c r="F71" s="37" t="s">
+        <v>111</v>
+      </c>
+      <c r="G71" s="27" t="s">
+        <v>321</v>
+      </c>
+      <c r="H71" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="I71" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="J71" s="40" t="s">
+        <v>77</v>
+      </c>
+      <c r="K71" s="40" t="s">
+        <v>320</v>
+      </c>
       <c r="L71" s="28"/>
       <c r="M71" s="28"/>
       <c r="N71" s="28"/>
       <c r="O71" s="28"/>
-      <c r="P71" s="25"/>
-      <c r="Q71" s="26"/>
+      <c r="P71" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q71" s="26" t="s">
+        <v>292</v>
+      </c>
       <c r="R71" s="34"/>
     </row>
     <row r="72" spans="1:18" s="18" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="36"/>
-      <c r="B72" s="27"/>
-      <c r="C72" s="43"/>
+      <c r="B72" s="27" t="s">
+        <v>293</v>
+      </c>
+      <c r="C72" s="43">
+        <v>11</v>
+      </c>
       <c r="D72" s="34"/>
-      <c r="E72" s="30"/>
-      <c r="F72" s="37"/>
-      <c r="G72" s="27"/>
-      <c r="H72" s="27"/>
-      <c r="I72" s="27"/>
-      <c r="J72" s="40"/>
-      <c r="K72" s="40"/>
+      <c r="E72" s="30" t="s">
+        <v>322</v>
+      </c>
+      <c r="F72" s="37" t="s">
+        <v>111</v>
+      </c>
+      <c r="G72" s="27" t="s">
+        <v>323</v>
+      </c>
+      <c r="H72" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="I72" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="J72" s="40" t="s">
+        <v>355</v>
+      </c>
+      <c r="K72" s="40" t="s">
+        <v>324</v>
+      </c>
       <c r="L72" s="28"/>
       <c r="M72" s="28"/>
       <c r="N72" s="28"/>
       <c r="O72" s="28"/>
-      <c r="P72" s="25"/>
-      <c r="Q72" s="26"/>
+      <c r="P72" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q72" s="26" t="s">
+        <v>292</v>
+      </c>
       <c r="R72" s="34"/>
     </row>
     <row r="73" spans="1:18" s="18" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="36"/>
-      <c r="B73" s="27"/>
-      <c r="C73" s="43"/>
+      <c r="B73" s="27" t="s">
+        <v>293</v>
+      </c>
+      <c r="C73" s="43">
+        <v>11</v>
+      </c>
       <c r="D73" s="34"/>
-      <c r="E73" s="39"/>
-      <c r="F73" s="37"/>
-      <c r="G73" s="27"/>
-      <c r="H73" s="27"/>
-      <c r="I73" s="27"/>
-      <c r="J73" s="40"/>
-      <c r="K73" s="40"/>
+      <c r="E73" s="39" t="s">
+        <v>325</v>
+      </c>
+      <c r="F73" s="37" t="s">
+        <v>111</v>
+      </c>
+      <c r="G73" s="27" t="s">
+        <v>326</v>
+      </c>
+      <c r="H73" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="I73" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="J73" s="40" t="s">
+        <v>67</v>
+      </c>
+      <c r="K73" s="40" t="s">
+        <v>327</v>
+      </c>
       <c r="L73" s="28"/>
       <c r="M73" s="28"/>
       <c r="N73" s="28"/>
       <c r="O73" s="28"/>
-      <c r="P73" s="25"/>
-      <c r="Q73" s="26"/>
+      <c r="P73" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q73" s="26" t="s">
+        <v>292</v>
+      </c>
       <c r="R73" s="34"/>
     </row>
     <row r="74" spans="1:18" s="18" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="36"/>
-      <c r="B74" s="27"/>
-      <c r="C74" s="43"/>
+      <c r="B74" s="27" t="s">
+        <v>293</v>
+      </c>
+      <c r="C74" s="43">
+        <v>11</v>
+      </c>
       <c r="D74" s="34"/>
-      <c r="E74" s="39"/>
-      <c r="F74" s="37"/>
-      <c r="G74" s="28"/>
-      <c r="H74" s="27"/>
-      <c r="I74" s="27"/>
-      <c r="J74" s="54"/>
-      <c r="K74" s="54"/>
+      <c r="E74" s="39" t="s">
+        <v>328</v>
+      </c>
+      <c r="F74" s="37" t="s">
+        <v>111</v>
+      </c>
+      <c r="G74" s="28" t="s">
+        <v>329</v>
+      </c>
+      <c r="H74" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="I74" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="J74" s="54" t="s">
+        <v>337</v>
+      </c>
+      <c r="K74" s="54" t="s">
+        <v>338</v>
+      </c>
       <c r="L74" s="28"/>
       <c r="M74" s="28"/>
       <c r="N74" s="28"/>
       <c r="O74" s="28"/>
-      <c r="P74" s="25"/>
-      <c r="Q74" s="26"/>
+      <c r="P74" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q74" s="26" t="s">
+        <v>292</v>
+      </c>
       <c r="R74" s="34"/>
     </row>
     <row r="75" spans="1:18" s="18" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="36"/>
-      <c r="B75" s="27"/>
-      <c r="C75" s="43"/>
+      <c r="B75" s="27" t="s">
+        <v>293</v>
+      </c>
+      <c r="C75" s="43">
+        <v>11</v>
+      </c>
       <c r="D75" s="34"/>
-      <c r="E75" s="39"/>
-      <c r="F75" s="37"/>
-      <c r="G75" s="27"/>
-      <c r="H75" s="27"/>
-      <c r="I75" s="27"/>
-      <c r="J75" s="54"/>
-      <c r="K75" s="54"/>
+      <c r="E75" s="39" t="s">
+        <v>331</v>
+      </c>
+      <c r="F75" s="37" t="s">
+        <v>111</v>
+      </c>
+      <c r="G75" s="27" t="s">
+        <v>332</v>
+      </c>
+      <c r="H75" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="I75" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="J75" s="54" t="s">
+        <v>334</v>
+      </c>
+      <c r="K75" s="54" t="s">
+        <v>335</v>
+      </c>
       <c r="L75" s="28"/>
       <c r="M75" s="28"/>
       <c r="N75" s="28"/>
       <c r="O75" s="28"/>
-      <c r="P75" s="25"/>
-      <c r="Q75" s="26"/>
+      <c r="P75" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q75" s="26" t="s">
+        <v>292</v>
+      </c>
       <c r="R75" s="34"/>
     </row>
     <row r="76" spans="1:18" s="18" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="69"/>
-      <c r="B76" s="55"/>
-      <c r="C76" s="71"/>
+      <c r="B76" s="55" t="s">
+        <v>293</v>
+      </c>
+      <c r="C76" s="71">
+        <v>11</v>
+      </c>
       <c r="D76" s="70"/>
-      <c r="E76" s="55"/>
-      <c r="F76" s="32"/>
-      <c r="G76" s="55"/>
-      <c r="H76" s="55"/>
-      <c r="I76" s="55"/>
-      <c r="J76" s="40"/>
-      <c r="K76" s="40"/>
+      <c r="E76" s="55" t="s">
+        <v>336</v>
+      </c>
+      <c r="F76" s="32" t="s">
+        <v>111</v>
+      </c>
+      <c r="G76" s="55" t="s">
+        <v>340</v>
+      </c>
+      <c r="H76" s="55" t="s">
+        <v>62</v>
+      </c>
+      <c r="I76" s="55" t="s">
+        <v>43</v>
+      </c>
+      <c r="J76" s="40" t="s">
+        <v>354</v>
+      </c>
+      <c r="K76" s="40" t="s">
+        <v>339</v>
+      </c>
       <c r="L76" s="60"/>
       <c r="M76" s="60"/>
       <c r="N76" s="60"/>
       <c r="O76" s="60"/>
-      <c r="P76" s="16"/>
-      <c r="Q76" s="80"/>
+      <c r="P76" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q76" s="80" t="s">
+        <v>292</v>
+      </c>
       <c r="R76" s="70"/>
     </row>
     <row r="77" spans="1:18" s="18" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="36"/>
-      <c r="B77" s="27"/>
-      <c r="C77" s="43"/>
+      <c r="B77" s="27" t="s">
+        <v>293</v>
+      </c>
+      <c r="C77" s="43">
+        <v>11</v>
+      </c>
       <c r="D77" s="34"/>
-      <c r="E77" s="39"/>
-      <c r="F77" s="37"/>
-      <c r="G77" s="27"/>
-      <c r="H77" s="27"/>
-      <c r="I77" s="27"/>
-      <c r="J77" s="54"/>
-      <c r="K77" s="54"/>
+      <c r="E77" s="39" t="s">
+        <v>341</v>
+      </c>
+      <c r="F77" s="37" t="s">
+        <v>111</v>
+      </c>
+      <c r="G77" s="27" t="s">
+        <v>342</v>
+      </c>
+      <c r="H77" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="I77" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="J77" s="54" t="s">
+        <v>353</v>
+      </c>
+      <c r="K77" s="54" t="s">
+        <v>338</v>
+      </c>
       <c r="L77" s="28"/>
       <c r="M77" s="28"/>
       <c r="N77" s="28"/>
       <c r="O77" s="28"/>
-      <c r="P77" s="25"/>
-      <c r="Q77" s="26"/>
+      <c r="P77" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q77" s="26" t="s">
+        <v>292</v>
+      </c>
       <c r="R77" s="34"/>
     </row>
     <row r="78" spans="1:18" s="18" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="36"/>
-      <c r="B78" s="27"/>
-      <c r="C78" s="43"/>
+      <c r="B78" s="27" t="s">
+        <v>293</v>
+      </c>
+      <c r="C78" s="43">
+        <v>11</v>
+      </c>
       <c r="D78" s="34"/>
-      <c r="E78" s="39"/>
-      <c r="F78" s="37"/>
-      <c r="G78" s="27"/>
-      <c r="H78" s="27"/>
-      <c r="I78" s="27"/>
-      <c r="J78" s="54"/>
-      <c r="K78" s="54"/>
+      <c r="E78" s="39" t="s">
+        <v>344</v>
+      </c>
+      <c r="F78" s="37" t="s">
+        <v>111</v>
+      </c>
+      <c r="G78" s="27" t="s">
+        <v>346</v>
+      </c>
+      <c r="H78" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="I78" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="J78" s="54" t="s">
+        <v>343</v>
+      </c>
+      <c r="K78" s="54" t="s">
+        <v>343</v>
+      </c>
       <c r="L78" s="28"/>
       <c r="M78" s="28"/>
       <c r="N78" s="28"/>
       <c r="O78" s="28"/>
-      <c r="P78" s="25"/>
-      <c r="Q78" s="26"/>
+      <c r="P78" s="25" t="s">
+        <v>330</v>
+      </c>
+      <c r="Q78" s="26" t="s">
+        <v>292</v>
+      </c>
       <c r="R78" s="34"/>
     </row>
     <row r="79" spans="1:18" s="18" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="36"/>
-      <c r="B79" s="27"/>
-      <c r="C79" s="43"/>
+      <c r="B79" s="27" t="s">
+        <v>293</v>
+      </c>
+      <c r="C79" s="43">
+        <v>11</v>
+      </c>
       <c r="D79" s="34"/>
-      <c r="E79" s="34"/>
-      <c r="F79" s="37"/>
-      <c r="G79" s="27"/>
-      <c r="H79" s="27"/>
-      <c r="I79" s="27"/>
-      <c r="J79" s="40"/>
-      <c r="K79" s="40"/>
+      <c r="E79" s="34" t="s">
+        <v>345</v>
+      </c>
+      <c r="F79" s="37" t="s">
+        <v>111</v>
+      </c>
+      <c r="G79" s="27" t="s">
+        <v>347</v>
+      </c>
+      <c r="H79" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="I79" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="J79" s="40" t="s">
+        <v>352</v>
+      </c>
+      <c r="K79" s="40" t="s">
+        <v>348</v>
+      </c>
       <c r="L79" s="28"/>
       <c r="M79" s="28"/>
       <c r="N79" s="28"/>
       <c r="O79" s="28"/>
-      <c r="P79" s="25"/>
-      <c r="Q79" s="26"/>
+      <c r="P79" s="25" t="s">
+        <v>330</v>
+      </c>
+      <c r="Q79" s="26" t="s">
+        <v>292</v>
+      </c>
       <c r="R79" s="34"/>
     </row>
     <row r="80" spans="1:18" s="18" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="36"/>
-      <c r="B80" s="27"/>
-      <c r="C80" s="43"/>
+      <c r="B80" s="27" t="s">
+        <v>293</v>
+      </c>
+      <c r="C80" s="43">
+        <v>11</v>
+      </c>
       <c r="D80" s="34"/>
-      <c r="E80" s="27"/>
-      <c r="F80" s="37"/>
-      <c r="G80" s="27"/>
-      <c r="H80" s="27"/>
-      <c r="I80" s="27"/>
-      <c r="J80" s="54"/>
-      <c r="K80" s="54"/>
+      <c r="E80" s="27" t="s">
+        <v>349</v>
+      </c>
+      <c r="F80" s="37" t="s">
+        <v>111</v>
+      </c>
+      <c r="G80" s="27" t="s">
+        <v>350</v>
+      </c>
+      <c r="H80" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="I80" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="J80" s="54" t="s">
+        <v>351</v>
+      </c>
+      <c r="K80" s="54" t="s">
+        <v>356</v>
+      </c>
       <c r="L80" s="28"/>
       <c r="M80" s="28"/>
       <c r="N80" s="28"/>
       <c r="O80" s="28"/>
-      <c r="P80" s="25"/>
-      <c r="Q80" s="26"/>
+      <c r="P80" s="25" t="s">
+        <v>330</v>
+      </c>
+      <c r="Q80" s="26" t="s">
+        <v>292</v>
+      </c>
       <c r="R80" s="34"/>
     </row>
     <row r="81" spans="1:18" s="18" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -5410,8 +6010,12 @@
       <c r="M81" s="60"/>
       <c r="N81" s="60"/>
       <c r="O81" s="60"/>
-      <c r="P81" s="16"/>
-      <c r="Q81" s="80"/>
+      <c r="P81" s="25" t="s">
+        <v>330</v>
+      </c>
+      <c r="Q81" s="80" t="s">
+        <v>292</v>
+      </c>
       <c r="R81" s="70"/>
     </row>
     <row r="82" spans="1:18" s="18" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -20873,10 +21477,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -20901,15 +21505,26 @@
         <v>213</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>292</v>
+      </c>
+      <c r="B3" t="s">
+        <v>333</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -20962,24 +21577,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{30E84F96-43E5-4C3A-8E0E-76AD01F7D6A1}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{56277F14-5102-450B-9F74-CC1199F0A7EB}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -21000,9 +21606,15 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{56277F14-5102-450B-9F74-CC1199F0A7EB}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{30E84F96-43E5-4C3A-8E0E-76AD01F7D6A1}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>